<commit_message>
added diagnostics and more in detail summaries of results
</commit_message>
<xml_diff>
--- a/RESULTS/Table_2_det_function.xlsx
+++ b/RESULTS/Table_2_det_function.xlsx
@@ -12,27 +12,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C-vM $p$-value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average detectability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">se(Average detectability)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delta AIC</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covariates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cramér von Mises p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p0 ± SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta_AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazard-rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seastate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.055 ± 0.0167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1041 ± 0.0255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1033 ± 0.0262</t>
   </si>
   <si>
     <t xml:space="preserve">m1</t>
@@ -41,19 +71,19 @@
     <t xml:space="preserve">Half-normal</t>
   </si>
   <si>
-    <t xml:space="preserve">~1</t>
+    <t xml:space="preserve">0.4008 ± 0.0261</t>
   </si>
   <si>
     <t xml:space="preserve">m3</t>
   </si>
   <si>
-    <t xml:space="preserve">~subj</t>
+    <t xml:space="preserve">0.3911 ± 0.0301</t>
   </si>
   <si>
     <t xml:space="preserve">m2</t>
   </si>
   <si>
-    <t xml:space="preserve">~seastate</t>
+    <t xml:space="preserve">0.3933 ± 0.0279</t>
   </si>
 </sst>
 </file>
@@ -419,13 +449,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00554479812965869</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.400778652185819</v>
+        <v>0.1256</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0260943995120859</v>
+        <v>1365.85630288711</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -433,48 +463,117 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00677700351619903</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.391066566289856</v>
+        <v>0.0897</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0300842180659558</v>
+        <v>1371.1122000113</v>
       </c>
       <c r="G3" t="n">
-        <v>1.41392869811011</v>
+        <v>5.25589712419014</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0075753014417308</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.393253103367021</v>
+        <v>0.0959</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0279241102053832</v>
+        <v>1375.05030008077</v>
       </c>
       <c r="G4" t="n">
-        <v>2.62762301262001</v>
+        <v>9.19399719366015</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0055</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1382.52054414473</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16.66424125762</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0068</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1383.93447284284</v>
+      </c>
+      <c r="G6" t="n">
+        <v>18.0781699557301</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0076</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1385.14816715735</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.29186427024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified output and fixed error in confidence interval for abundance summary
</commit_message>
<xml_diff>
--- a/RESULTS/Table_2_det_function.xlsx
+++ b/RESULTS/Table_2_det_function.xlsx
@@ -455,7 +455,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>1365.85630288711</v>
+        <v>1365.86</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -478,10 +478,10 @@
         <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>1371.1122000113</v>
+        <v>1371.11</v>
       </c>
       <c r="G3" t="n">
-        <v>5.25589712419014</v>
+        <v>5.26</v>
       </c>
     </row>
     <row r="4">
@@ -501,10 +501,10 @@
         <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>1375.05030008077</v>
+        <v>1375.05</v>
       </c>
       <c r="G4" t="n">
-        <v>9.19399719366015</v>
+        <v>9.19</v>
       </c>
     </row>
     <row r="5">
@@ -524,10 +524,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>1382.52054414473</v>
+        <v>1382.52</v>
       </c>
       <c r="G5" t="n">
-        <v>16.66424125762</v>
+        <v>16.66</v>
       </c>
     </row>
     <row r="6">
@@ -547,10 +547,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="n">
-        <v>1383.93447284284</v>
+        <v>1383.93</v>
       </c>
       <c r="G6" t="n">
-        <v>18.0781699557301</v>
+        <v>18.08</v>
       </c>
     </row>
     <row r="7">
@@ -570,10 +570,10 @@
         <v>23</v>
       </c>
       <c r="F7" t="n">
-        <v>1385.14816715735</v>
+        <v>1385.15</v>
       </c>
       <c r="G7" t="n">
-        <v>19.29186427024</v>
+        <v>19.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>